<commit_message>
## Add more code
</commit_message>
<xml_diff>
--- a/TestData/Fate测试表.xlsx
+++ b/TestData/Fate测试表.xlsx
@@ -11,7 +11,7 @@
     <sheet name="护送" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
   <si>
     <t>FateID</t>
   </si>
@@ -377,6 +377,69 @@
   </si>
   <si>
     <t>FATE_ROUTE_W1F4_016</t>
+  </si>
+  <si>
+    <t>217</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>289</t>
+  </si>
+  <si>
+    <t>334</t>
+  </si>
+  <si>
+    <t>354</t>
+  </si>
+  <si>
+    <t>432</t>
+  </si>
+  <si>
+    <t>491</t>
+  </si>
+  <si>
+    <t>501</t>
+  </si>
+  <si>
+    <t>529</t>
+  </si>
+  <si>
+    <t>642</t>
+  </si>
+  <si>
+    <t>716</t>
+  </si>
+  <si>
+    <t>752</t>
+  </si>
+  <si>
+    <t>777</t>
+  </si>
+  <si>
+    <t>853</t>
+  </si>
+  <si>
+    <t>1120</t>
+  </si>
+  <si>
+    <t>1121</t>
+  </si>
+  <si>
+    <t>1173</t>
+  </si>
+  <si>
+    <t>1270</t>
+  </si>
+  <si>
+    <t>1429</t>
+  </si>
+  <si>
+    <t>1434</t>
+  </si>
+  <si>
+    <t>1595</t>
   </si>
 </sst>
 </file>
@@ -844,162 +907,162 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" applyNumberFormat="1" fontId="0" applyFont="0" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" applyNumberFormat="1" fontId="0" applyFont="0" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" applyNumberFormat="1" fontId="0" applyFont="0" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" applyNumberFormat="1" fontId="0" applyFont="0" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" applyNumberFormat="1" fontId="0" applyFont="0" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="1" applyFont="1" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="2" applyFont="1" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="0" applyFont="0" fillId="2" applyFill="1" borderId="1" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="3" applyFont="1" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="4" applyFont="1" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="5" applyFont="1" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="6" applyFont="1" fillId="0" applyFill="0" borderId="2" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="7" applyFont="1" fillId="0" applyFill="0" borderId="2" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="8" applyFont="1" fillId="0" applyFill="0" borderId="3" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="8" applyFont="1" fillId="0" applyFill="0" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="9" applyFont="1" fillId="3" applyFill="1" borderId="4" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="10" applyFont="1" fillId="4" applyFill="1" borderId="5" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="11" applyFont="1" fillId="4" applyFill="1" borderId="4" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="12" applyFont="1" fillId="5" applyFill="1" borderId="6" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="13" applyFont="1" fillId="0" applyFill="0" borderId="7" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="14" applyFont="1" fillId="0" applyFill="0" borderId="8" applyBorder="1" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="15" applyFont="1" fillId="6" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="16" applyFont="1" fillId="7" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="17" applyFont="1" fillId="8" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="18" applyFont="1" fillId="9" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="10" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="11" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="18" applyFont="1" fillId="12" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="18" applyFont="1" fillId="13" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="14" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="15" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="18" applyFont="1" fillId="16" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="18" applyFont="1" fillId="17" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="18" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="19" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="18" applyFont="1" fillId="20" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="18" applyFont="1" fillId="21" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="22" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="23" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="18" applyFont="1" fillId="24" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="18" applyFont="1" fillId="25" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="26" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="27" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="18" applyFont="1" fillId="28" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="18" applyFont="1" fillId="29" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="30" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="19" applyFont="1" fillId="31" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="18" applyFont="1" fillId="32" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1321,20 +1384,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="12" width="9" style="1"/>
-    <col min="13" max="13" width="19.125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5" style="1" customWidth="1"/>
-    <col min="15" max="15" width="23.75" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9" style="1"/>
-    <col min="17" max="17" width="29.375" style="1" customWidth="1"/>
-    <col min="18" max="20" width="9" style="1"/>
-    <col min="21" max="21" width="18.25" style="1" customWidth="1"/>
-    <col min="22" max="23" width="9" style="1"/>
-    <col min="24" max="24" width="18.25" style="1" customWidth="1"/>
-    <col min="25" max="16384" width="9" style="1"/>
+    <col min="1" max="12" width="9" customWidth="1" style="1"/>
+    <col min="13" max="13" width="19.125" customWidth="1" style="1"/>
+    <col min="14" max="14" width="11.5" customWidth="1" style="1"/>
+    <col min="15" max="15" width="23.75" customWidth="1" style="1"/>
+    <col min="16" max="16" width="9" customWidth="1" style="1"/>
+    <col min="17" max="17" width="29.375" customWidth="1" style="1"/>
+    <col min="18" max="20" width="9" customWidth="1" style="1"/>
+    <col min="21" max="21" width="18.25" customWidth="1" style="1"/>
+    <col min="22" max="23" width="9" customWidth="1" style="1"/>
+    <col min="24" max="24" width="18.25" customWidth="1" style="1"/>
+    <col min="25" max="16384" width="9" customWidth="1" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1417,7 +1480,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -1500,7 +1563,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3">
       <c r="A3" s="1">
         <v>447</v>
       </c>
@@ -1572,7 +1635,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AL4"/>
+  <dimension ref="A1:AL24"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
       <selection activeCell="H33" sqref="H33"/>
@@ -1580,31 +1643,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3"/>
   <cols>
-    <col min="1" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="26" style="1" customWidth="1"/>
-    <col min="7" max="9" width="9" style="1"/>
-    <col min="10" max="10" width="26" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="19.25" style="1" customWidth="1"/>
-    <col min="13" max="13" width="16" style="1" customWidth="1"/>
-    <col min="14" max="14" width="26" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.625" style="1" customWidth="1"/>
-    <col min="16" max="17" width="9" style="1"/>
-    <col min="18" max="18" width="26" style="1" customWidth="1"/>
-    <col min="19" max="21" width="9" style="1"/>
-    <col min="22" max="22" width="26" style="1" customWidth="1"/>
-    <col min="23" max="25" width="9" style="1"/>
-    <col min="26" max="26" width="26" style="1" customWidth="1"/>
-    <col min="27" max="29" width="9" style="1"/>
-    <col min="30" max="30" width="13" style="1" customWidth="1"/>
-    <col min="31" max="33" width="9" style="1"/>
-    <col min="34" max="34" width="13" style="1" customWidth="1"/>
-    <col min="35" max="37" width="9" style="1"/>
-    <col min="38" max="38" width="13" style="1" customWidth="1"/>
-    <col min="39" max="16384" width="9" style="1"/>
+    <col min="1" max="5" width="9" customWidth="1" style="1"/>
+    <col min="6" max="6" width="26" customWidth="1" style="1"/>
+    <col min="7" max="9" width="9" customWidth="1" style="1"/>
+    <col min="10" max="10" width="26" customWidth="1" style="1"/>
+    <col min="11" max="11" width="17.875" customWidth="1" style="1"/>
+    <col min="12" max="12" width="19.25" customWidth="1" style="1"/>
+    <col min="13" max="13" width="16" customWidth="1" style="1"/>
+    <col min="14" max="14" width="26" customWidth="1" style="1"/>
+    <col min="15" max="15" width="12.625" customWidth="1" style="1"/>
+    <col min="16" max="17" width="9" customWidth="1" style="1"/>
+    <col min="18" max="18" width="26" customWidth="1" style="1"/>
+    <col min="19" max="21" width="9" customWidth="1" style="1"/>
+    <col min="22" max="22" width="26" customWidth="1" style="1"/>
+    <col min="23" max="25" width="9" customWidth="1" style="1"/>
+    <col min="26" max="26" width="26" customWidth="1" style="1"/>
+    <col min="27" max="29" width="9" customWidth="1" style="1"/>
+    <col min="30" max="30" width="13" customWidth="1" style="1"/>
+    <col min="31" max="33" width="9" customWidth="1" style="1"/>
+    <col min="34" max="34" width="13" customWidth="1" style="1"/>
+    <col min="35" max="37" width="9" customWidth="1" style="1"/>
+    <col min="38" max="38" width="13" customWidth="1" style="1"/>
+    <col min="39" max="16384" width="9" customWidth="1" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:38">
+    <row r="1">
       <c r="C1" s="2" t="s">
         <v>66</v>
       </c>
@@ -1660,7 +1723,7 @@
       <c r="AK1" s="2"/>
       <c r="AL1" s="2"/>
     </row>
-    <row r="2" spans="1:38">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1776,7 +1839,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:38">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1892,7 +1955,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4">
       <c r="A4" s="1">
         <v>434</v>
       </c>
@@ -1933,8 +1996,2328 @@
         <v>4101897</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL5" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL6" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK7" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL7" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK8" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL8" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL9" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL10" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL11" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL12" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="X13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK13" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL13" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="X14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL14" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL15" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL16" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="X17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL17" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="X18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL18" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="X19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK19" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL19" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="X20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK20" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL20" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="X21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL21" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="X22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL22" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="X23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL23" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="U24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="V24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="X24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL24" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="K1:N1"/>
@@ -1954,7 +4337,6 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>

</xml_diff>

<commit_message>
## Ver 2.2.1 , fix bug
</commit_message>
<xml_diff>
--- a/TestData/Fate测试表.xlsx
+++ b/TestData/Fate测试表.xlsx
@@ -16,7 +16,7 @@
     <sheet name="护送" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="179">
   <si>
     <t>路径点0</t>
   </si>
@@ -192,6 +192,54 @@
     <t>移动前行动</t>
   </si>
   <si>
+    <t>217</t>
+  </si>
+  <si>
+    <t>F1F2_014</t>
+  </si>
+  <si>
+    <t>4164925</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>289</t>
+  </si>
+  <si>
+    <t>S1F4_002</t>
+  </si>
+  <si>
+    <t>4176053</t>
+  </si>
+  <si>
+    <t>334</t>
+  </si>
+  <si>
+    <t>S1F3_024</t>
+  </si>
+  <si>
+    <t>4165302</t>
+  </si>
+  <si>
+    <t>354</t>
+  </si>
+  <si>
+    <t>W1F1_015</t>
+  </si>
+  <si>
+    <t>4176117</t>
+  </si>
+  <si>
+    <t>432</t>
+  </si>
+  <si>
+    <t>W1F4_014</t>
+  </si>
+  <si>
+    <t>4172489</t>
+  </si>
+  <si>
     <t>434</t>
   </si>
   <si>
@@ -201,10 +249,139 @@
     <t>4101798</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t/>
+    <t>491</t>
+  </si>
+  <si>
+    <t>R1F1_032</t>
+  </si>
+  <si>
+    <t>4317651</t>
+  </si>
+  <si>
+    <t>501</t>
+  </si>
+  <si>
+    <t>R1F1_042</t>
+  </si>
+  <si>
+    <t>4304056</t>
+  </si>
+  <si>
+    <t>529</t>
+  </si>
+  <si>
+    <t>L1F1_020</t>
+  </si>
+  <si>
+    <t>4300283</t>
+  </si>
+  <si>
+    <t>642</t>
+  </si>
+  <si>
+    <t>W1F5_019</t>
+  </si>
+  <si>
+    <t>4322757</t>
+  </si>
+  <si>
+    <t>716</t>
+  </si>
+  <si>
+    <t>W1T1_HALLOWEEN_2014_01</t>
+  </si>
+  <si>
+    <t>5033053</t>
+  </si>
+  <si>
+    <t>752</t>
+  </si>
+  <si>
+    <t>D2F3_028</t>
+  </si>
+  <si>
+    <t>5923771</t>
+  </si>
+  <si>
+    <t>777</t>
+  </si>
+  <si>
+    <t>D2F2_022</t>
+  </si>
+  <si>
+    <t>5912759</t>
+  </si>
+  <si>
+    <t>853</t>
+  </si>
+  <si>
+    <t>A2F1_015</t>
+  </si>
+  <si>
+    <t>5935441</t>
+  </si>
+  <si>
+    <t>1120</t>
+  </si>
+  <si>
+    <t>G3F1_011</t>
+  </si>
+  <si>
+    <t>6930892</t>
+  </si>
+  <si>
+    <t>1121</t>
+  </si>
+  <si>
+    <t>G3F1_012</t>
+  </si>
+  <si>
+    <t>6874028</t>
+  </si>
+  <si>
+    <t>1173</t>
+  </si>
+  <si>
+    <t>G3F2_001</t>
+  </si>
+  <si>
+    <t>6937498</t>
+  </si>
+  <si>
+    <t>1270</t>
+  </si>
+  <si>
+    <t>E3F3_029</t>
+  </si>
+  <si>
+    <t>6982854</t>
+  </si>
+  <si>
+    <t>1429</t>
+  </si>
+  <si>
+    <t>N4F6_004</t>
+  </si>
+  <si>
+    <t>8003842</t>
+  </si>
+  <si>
+    <t>1434</t>
+  </si>
+  <si>
+    <t>N4F6_009</t>
+  </si>
+  <si>
+    <t>8006210</t>
+  </si>
+  <si>
+    <t>1595</t>
+  </si>
+  <si>
+    <t>F1T2_イースター_2020_後半</t>
+  </si>
+  <si>
+    <t>8283030</t>
   </si>
   <si>
     <t>版本</t>
@@ -400,7 +577,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,7 +605,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -435,10 +613,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -716,204 +894,204 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="12" width="9" style="1" customWidth="1"/>
-    <col min="13" max="13" width="19.125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5" style="1" customWidth="1"/>
-    <col min="15" max="15" width="23.75" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9" style="1" customWidth="1"/>
-    <col min="17" max="17" width="29.375" style="1" customWidth="1"/>
-    <col min="18" max="20" width="9" style="1" customWidth="1"/>
-    <col min="21" max="21" width="18.25" style="1" customWidth="1"/>
-    <col min="22" max="23" width="9" style="1" customWidth="1"/>
-    <col min="24" max="24" width="18.25" style="1" customWidth="1"/>
-    <col min="25" max="27" width="9" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="9" style="1"/>
+    <col min="1" max="12" width="9" customWidth="1" style="1"/>
+    <col min="13" max="13" width="19.125" customWidth="1" style="1"/>
+    <col min="14" max="14" width="11.5" customWidth="1" style="1"/>
+    <col min="15" max="15" width="23.75" customWidth="1" style="1"/>
+    <col min="16" max="16" width="9" customWidth="1" style="1"/>
+    <col min="17" max="17" width="29.375" customWidth="1" style="1"/>
+    <col min="18" max="20" width="9" customWidth="1" style="1"/>
+    <col min="21" max="21" width="18.25" customWidth="1" style="1"/>
+    <col min="22" max="23" width="9" customWidth="1" style="1"/>
+    <col min="24" max="24" width="18.25" customWidth="1" style="1"/>
+    <col min="25" max="27" width="9" customWidth="1" style="1"/>
+    <col min="28" max="16384" width="9" customWidth="1" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>116</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>59</v>
+        <v>118</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>60</v>
+        <v>119</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>61</v>
+        <v>120</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>62</v>
+        <v>121</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>63</v>
+        <v>122</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>64</v>
+        <v>123</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>65</v>
+        <v>124</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>66</v>
+        <v>125</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>67</v>
+        <v>126</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>68</v>
+        <v>127</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>69</v>
+        <v>128</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>70</v>
+        <v>129</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>71</v>
+        <v>130</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>72</v>
+        <v>131</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>73</v>
+        <v>132</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>74</v>
+        <v>133</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>75</v>
+        <v>134</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>76</v>
+        <v>135</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>77</v>
+        <v>136</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>78</v>
+        <v>137</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>79</v>
+        <v>138</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>80</v>
+        <v>139</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>81</v>
+        <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="2">
       <c r="A2" s="1" t="s">
-        <v>82</v>
+        <v>141</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>83</v>
+        <v>142</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>84</v>
+        <v>143</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>85</v>
+        <v>144</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>86</v>
+        <v>145</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>87</v>
+        <v>146</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>88</v>
+        <v>147</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>89</v>
+        <v>148</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>90</v>
+        <v>149</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>91</v>
+        <v>150</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>92</v>
+        <v>151</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>93</v>
+        <v>152</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>94</v>
+        <v>153</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>95</v>
+        <v>154</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>96</v>
+        <v>155</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>97</v>
+        <v>156</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>98</v>
+        <v>157</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>99</v>
+        <v>158</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>100</v>
+        <v>159</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>101</v>
+        <v>160</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>102</v>
+        <v>161</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>103</v>
+        <v>162</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>104</v>
+        <v>163</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>105</v>
+        <v>164</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>106</v>
+        <v>165</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>107</v>
+        <v>166</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="3">
       <c r="A3" s="1">
         <v>447</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>108</v>
+        <v>167</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>109</v>
+        <v>168</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>110</v>
+        <v>169</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>111</v>
+        <v>170</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>112</v>
+        <v>171</v>
       </c>
       <c r="G3" s="1">
         <v>15</v>
@@ -937,37 +1115,38 @@
         <v>30001208</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>113</v>
+        <v>172</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>114</v>
+        <v>173</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>115</v>
+        <v>174</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>116</v>
+        <v>175</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>117</v>
+        <v>176</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>118</v>
+        <v>177</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>119</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL4"/>
+  <dimension ref="A1:AL24"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD61"/>
@@ -975,34 +1154,34 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.625" style="1" customWidth="1"/>
-    <col min="3" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26" style="1" customWidth="1"/>
-    <col min="7" max="9" width="9" style="1" customWidth="1"/>
-    <col min="10" max="10" width="26" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="19.25" style="1" customWidth="1"/>
-    <col min="13" max="13" width="16" style="1" customWidth="1"/>
-    <col min="14" max="14" width="26" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.625" style="1" customWidth="1"/>
-    <col min="16" max="17" width="9" style="1" customWidth="1"/>
-    <col min="18" max="18" width="26" style="1" customWidth="1"/>
-    <col min="19" max="21" width="9" style="1" customWidth="1"/>
-    <col min="22" max="22" width="26" style="1" customWidth="1"/>
-    <col min="23" max="25" width="9" style="1" customWidth="1"/>
-    <col min="26" max="26" width="26" style="1" customWidth="1"/>
-    <col min="27" max="29" width="9" style="1" customWidth="1"/>
-    <col min="30" max="30" width="13" style="1" customWidth="1"/>
-    <col min="31" max="33" width="9" style="1" customWidth="1"/>
-    <col min="34" max="34" width="13" style="1" customWidth="1"/>
-    <col min="35" max="37" width="9" style="1" customWidth="1"/>
-    <col min="38" max="38" width="13" style="1" customWidth="1"/>
-    <col min="39" max="41" width="9" style="1" customWidth="1"/>
-    <col min="42" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="9" customWidth="1" style="1"/>
+    <col min="2" max="2" width="13.625" customWidth="1" style="1"/>
+    <col min="3" max="5" width="9" customWidth="1" style="1"/>
+    <col min="6" max="6" width="26" customWidth="1" style="1"/>
+    <col min="7" max="9" width="9" customWidth="1" style="1"/>
+    <col min="10" max="10" width="26" customWidth="1" style="1"/>
+    <col min="11" max="11" width="17.875" customWidth="1" style="1"/>
+    <col min="12" max="12" width="19.25" customWidth="1" style="1"/>
+    <col min="13" max="13" width="16" customWidth="1" style="1"/>
+    <col min="14" max="14" width="26" customWidth="1" style="1"/>
+    <col min="15" max="15" width="12.625" customWidth="1" style="1"/>
+    <col min="16" max="17" width="9" customWidth="1" style="1"/>
+    <col min="18" max="18" width="26" customWidth="1" style="1"/>
+    <col min="19" max="21" width="9" customWidth="1" style="1"/>
+    <col min="22" max="22" width="26" customWidth="1" style="1"/>
+    <col min="23" max="25" width="9" customWidth="1" style="1"/>
+    <col min="26" max="26" width="26" customWidth="1" style="1"/>
+    <col min="27" max="29" width="9" customWidth="1" style="1"/>
+    <col min="30" max="30" width="13" customWidth="1" style="1"/>
+    <col min="31" max="33" width="9" customWidth="1" style="1"/>
+    <col min="34" max="34" width="13" customWidth="1" style="1"/>
+    <col min="35" max="37" width="9" customWidth="1" style="1"/>
+    <col min="38" max="38" width="13" customWidth="1" style="1"/>
+    <col min="39" max="41" width="9" customWidth="1" style="1"/>
+    <col min="42" max="16384" width="9" customWidth="1" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="1">
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1058,7 +1237,7 @@
       <c r="AK1" s="2"/>
       <c r="AL1" s="2"/>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1174,7 +1353,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1290,7 +1469,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="4">
       <c r="A4" s="1" t="s">
         <v>52</v>
       </c>
@@ -1304,110 +1483,2430 @@
         <v>55</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AD4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AE4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AG4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AH4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AJ4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AK4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AL4" s="1" t="s">
-        <v>56</v>
+      <c r="B5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL5" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL6" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL7" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL8" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL9" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL10" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL11" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL12" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL13" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL14" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL15" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL16" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL17" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL18" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL19" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL20" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL21" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL22" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL23" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="X24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AJ24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL24" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells>
     <mergeCell ref="W1:Z1"/>
     <mergeCell ref="AA1:AD1"/>
     <mergeCell ref="AE1:AH1"/>
@@ -1421,12 +3920,12 @@
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1435,5 +3934,6 @@
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
## Ver 2.2.3 , Add new function for config multi source data
</commit_message>
<xml_diff>
--- a/TestData/Fate测试表.xlsx
+++ b/TestData/Fate测试表.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="17925" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="17925" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="主流程" sheetId="2" r:id="rId1"/>
     <sheet name="护送" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="NPC测试" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913" fullCalcOnLoad="1"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="213">
   <si>
     <t>路径点0</t>
   </si>
@@ -382,6 +383,108 @@
   </si>
   <si>
     <t>8283030</t>
+  </si>
+  <si>
+    <t>#key</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>JLabel</t>
+  </si>
+  <si>
+    <t>#Key</t>
+  </si>
+  <si>
+    <t>keyAlias</t>
+  </si>
+  <si>
+    <t>keyDevcode</t>
+  </si>
+  <si>
+    <t>364</t>
+  </si>
+  <si>
+    <t>護衛テスト敵001</t>
+  </si>
+  <si>
+    <t>678</t>
+  </si>
+  <si>
+    <t>W1F4_014_敵_001_001</t>
+  </si>
+  <si>
+    <t>776</t>
+  </si>
+  <si>
+    <t>S1F3_024_敵_001_001</t>
+  </si>
+  <si>
+    <t>825</t>
+  </si>
+  <si>
+    <t>S1F4_002_敵_001_001</t>
+  </si>
+  <si>
+    <t>831</t>
+  </si>
+  <si>
+    <t>W1F1_015_敵_001_001</t>
+  </si>
+  <si>
+    <t>1756</t>
+  </si>
+  <si>
+    <t>W1T1_HALLOWEEN_2014_01_味方NPC_001</t>
+  </si>
+  <si>
+    <t>1893</t>
+  </si>
+  <si>
+    <t>D2F2_022_敵_001_001</t>
+  </si>
+  <si>
+    <t>2163</t>
+  </si>
+  <si>
+    <t>A2F1_015_敵_001</t>
+  </si>
+  <si>
+    <t>3018</t>
+  </si>
+  <si>
+    <t>G3F1_011_敵_001</t>
+  </si>
+  <si>
+    <t>3428</t>
+  </si>
+  <si>
+    <t>G3F2_001_敵_001</t>
+  </si>
+  <si>
+    <t>3909</t>
+  </si>
+  <si>
+    <t>E3F3_029_敵_001</t>
+  </si>
+  <si>
+    <t>4930</t>
+  </si>
+  <si>
+    <t>N4F6_004_敵_001</t>
+  </si>
+  <si>
+    <t>4936</t>
+  </si>
+  <si>
+    <t>N4F6_009_敵_001</t>
+  </si>
+  <si>
+    <t>5867</t>
+  </si>
+  <si>
+    <t>F1T2_イースター_2020_後半_配り対象_A_001</t>
   </si>
   <si>
     <t>版本</t>
@@ -609,11 +712,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -889,7 +995,7 @@
   <dimension ref="A1:AA3"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="AA17" sqref="AA17"/>
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -904,8 +1010,8 @@
     <col min="21" max="21" width="18.25" customWidth="1" style="1"/>
     <col min="22" max="23" width="9" customWidth="1" style="1"/>
     <col min="24" max="24" width="18.25" customWidth="1" style="1"/>
-    <col min="25" max="27" width="9" customWidth="1" style="1"/>
-    <col min="28" max="16384" width="9" customWidth="1" style="1"/>
+    <col min="25" max="30" width="9" customWidth="1" style="1"/>
+    <col min="31" max="16384" width="9" customWidth="1" style="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -913,165 +1019,165 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>117</v>
+        <v>151</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>119</v>
+        <v>153</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>120</v>
+        <v>154</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>121</v>
+        <v>155</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>124</v>
+        <v>158</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>125</v>
+        <v>159</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>126</v>
+        <v>160</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>127</v>
+        <v>161</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>128</v>
+        <v>162</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>129</v>
+        <v>163</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>130</v>
+        <v>164</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>131</v>
+        <v>165</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>132</v>
+        <v>166</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>133</v>
+        <v>167</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>136</v>
+        <v>170</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>138</v>
+        <v>172</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>139</v>
+        <v>173</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>141</v>
+        <v>175</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>142</v>
+        <v>176</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>144</v>
+        <v>178</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>145</v>
+        <v>179</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>147</v>
+        <v>181</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>149</v>
+        <v>183</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>150</v>
+        <v>184</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>151</v>
+        <v>185</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>152</v>
+        <v>186</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>153</v>
+        <v>187</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>154</v>
+        <v>188</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>155</v>
+        <v>189</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>156</v>
+        <v>190</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>157</v>
+        <v>191</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>158</v>
+        <v>192</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>160</v>
+        <v>194</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>161</v>
+        <v>195</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>162</v>
+        <v>196</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>163</v>
+        <v>197</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>164</v>
+        <v>198</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>165</v>
+        <v>199</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>166</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3">
@@ -1079,19 +1185,19 @@
         <v>447</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>167</v>
+        <v>201</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>168</v>
+        <v>202</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>169</v>
+        <v>203</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>170</v>
+        <v>204</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>171</v>
+        <v>205</v>
       </c>
       <c r="G3" s="1">
         <v>15</v>
@@ -1115,25 +1221,25 @@
         <v>30001208</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>172</v>
+        <v>206</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>173</v>
+        <v>207</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>174</v>
+        <v>208</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>175</v>
+        <v>209</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>176</v>
+        <v>210</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>177</v>
+        <v>211</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>178</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -1148,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL24"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD61"/>
+    <sheetView showFormulas="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1177,65 +1283,65 @@
     <col min="34" max="34" width="13" customWidth="1" style="1"/>
     <col min="35" max="37" width="9" customWidth="1" style="1"/>
     <col min="38" max="38" width="13" customWidth="1" style="1"/>
-    <col min="39" max="41" width="9" customWidth="1" style="1"/>
-    <col min="42" max="16384" width="9" customWidth="1" style="1"/>
+    <col min="39" max="44" width="9" customWidth="1" style="1"/>
+    <col min="45" max="16384" width="9" customWidth="1" style="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2" t="s">
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2" t="s">
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2" t="s">
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2" t="s">
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2" t="s">
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="2" t="s">
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AF1" s="2"/>
-      <c r="AG1" s="2"/>
-      <c r="AH1" s="2"/>
-      <c r="AI1" s="2" t="s">
+      <c r="AF1" s="3"/>
+      <c r="AG1" s="3"/>
+      <c r="AH1" s="3"/>
+      <c r="AI1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="AJ1" s="2"/>
-      <c r="AK1" s="2"/>
-      <c r="AL1" s="2"/>
+      <c r="AJ1" s="3"/>
+      <c r="AK1" s="3"/>
+      <c r="AL1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
@@ -3926,14 +4032,213 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="21.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K46" sqref="K46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="0" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
## Ver 2.2.3, add more code
</commit_message>
<xml_diff>
--- a/TestData/Fate测试表.xlsx
+++ b/TestData/Fate测试表.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="143">
   <si>
     <t>路径点0</t>
   </si>
@@ -196,195 +196,69 @@
     <t>217</t>
   </si>
   <si>
-    <t>F1F2_014</t>
-  </si>
-  <si>
-    <t>4164925</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
     <t>289</t>
   </si>
   <si>
-    <t>S1F4_002</t>
-  </si>
-  <si>
-    <t>4176053</t>
-  </si>
-  <si>
     <t>334</t>
   </si>
   <si>
-    <t>S1F3_024</t>
-  </si>
-  <si>
-    <t>4165302</t>
-  </si>
-  <si>
     <t>354</t>
   </si>
   <si>
-    <t>W1F1_015</t>
-  </si>
-  <si>
-    <t>4176117</t>
-  </si>
-  <si>
     <t>432</t>
   </si>
   <si>
-    <t>W1F4_014</t>
-  </si>
-  <si>
-    <t>4172489</t>
-  </si>
-  <si>
     <t>434</t>
   </si>
   <si>
-    <t>W1F4_016</t>
-  </si>
-  <si>
-    <t>4101798</t>
-  </si>
-  <si>
     <t>491</t>
   </si>
   <si>
-    <t>R1F1_032</t>
-  </si>
-  <si>
-    <t>4317651</t>
-  </si>
-  <si>
     <t>501</t>
   </si>
   <si>
-    <t>R1F1_042</t>
-  </si>
-  <si>
-    <t>4304056</t>
-  </si>
-  <si>
     <t>529</t>
   </si>
   <si>
-    <t>L1F1_020</t>
-  </si>
-  <si>
-    <t>4300283</t>
-  </si>
-  <si>
     <t>642</t>
   </si>
   <si>
-    <t>W1F5_019</t>
-  </si>
-  <si>
-    <t>4322757</t>
-  </si>
-  <si>
     <t>716</t>
   </si>
   <si>
-    <t>W1T1_HALLOWEEN_2014_01</t>
-  </si>
-  <si>
-    <t>5033053</t>
-  </si>
-  <si>
     <t>752</t>
   </si>
   <si>
-    <t>D2F3_028</t>
-  </si>
-  <si>
-    <t>5923771</t>
-  </si>
-  <si>
     <t>777</t>
   </si>
   <si>
-    <t>D2F2_022</t>
-  </si>
-  <si>
-    <t>5912759</t>
-  </si>
-  <si>
     <t>853</t>
   </si>
   <si>
-    <t>A2F1_015</t>
-  </si>
-  <si>
-    <t>5935441</t>
-  </si>
-  <si>
     <t>1120</t>
   </si>
   <si>
-    <t>G3F1_011</t>
-  </si>
-  <si>
-    <t>6930892</t>
-  </si>
-  <si>
     <t>1121</t>
   </si>
   <si>
-    <t>G3F1_012</t>
-  </si>
-  <si>
-    <t>6874028</t>
-  </si>
-  <si>
     <t>1173</t>
   </si>
   <si>
-    <t>G3F2_001</t>
-  </si>
-  <si>
-    <t>6937498</t>
-  </si>
-  <si>
     <t>1270</t>
   </si>
   <si>
-    <t>E3F3_029</t>
-  </si>
-  <si>
-    <t>6982854</t>
-  </si>
-  <si>
     <t>1429</t>
   </si>
   <si>
-    <t>N4F6_004</t>
-  </si>
-  <si>
-    <t>8003842</t>
-  </si>
-  <si>
     <t>1434</t>
   </si>
   <si>
-    <t>N4F6_009</t>
-  </si>
-  <si>
-    <t>8006210</t>
-  </si>
-  <si>
     <t>1595</t>
   </si>
   <si>
-    <t>F1T2_イースター_2020_後半</t>
-  </si>
-  <si>
-    <t>8283030</t>
-  </si>
-  <si>
     <t>#key</t>
   </si>
   <si>
@@ -401,90 +275,6 @@
   </si>
   <si>
     <t>keyDevcode</t>
-  </si>
-  <si>
-    <t>364</t>
-  </si>
-  <si>
-    <t>護衛テスト敵001</t>
-  </si>
-  <si>
-    <t>678</t>
-  </si>
-  <si>
-    <t>W1F4_014_敵_001_001</t>
-  </si>
-  <si>
-    <t>776</t>
-  </si>
-  <si>
-    <t>S1F3_024_敵_001_001</t>
-  </si>
-  <si>
-    <t>825</t>
-  </si>
-  <si>
-    <t>S1F4_002_敵_001_001</t>
-  </si>
-  <si>
-    <t>831</t>
-  </si>
-  <si>
-    <t>W1F1_015_敵_001_001</t>
-  </si>
-  <si>
-    <t>1756</t>
-  </si>
-  <si>
-    <t>W1T1_HALLOWEEN_2014_01_味方NPC_001</t>
-  </si>
-  <si>
-    <t>1893</t>
-  </si>
-  <si>
-    <t>D2F2_022_敵_001_001</t>
-  </si>
-  <si>
-    <t>2163</t>
-  </si>
-  <si>
-    <t>A2F1_015_敵_001</t>
-  </si>
-  <si>
-    <t>3018</t>
-  </si>
-  <si>
-    <t>G3F1_011_敵_001</t>
-  </si>
-  <si>
-    <t>3428</t>
-  </si>
-  <si>
-    <t>G3F2_001_敵_001</t>
-  </si>
-  <si>
-    <t>3909</t>
-  </si>
-  <si>
-    <t>E3F3_029_敵_001</t>
-  </si>
-  <si>
-    <t>4930</t>
-  </si>
-  <si>
-    <t>N4F6_004_敵_001</t>
-  </si>
-  <si>
-    <t>4936</t>
-  </si>
-  <si>
-    <t>N4F6_009_敵_001</t>
-  </si>
-  <si>
-    <t>5867</t>
-  </si>
-  <si>
-    <t>F1T2_イースター_2020_後半_配り対象_A_001</t>
   </si>
   <si>
     <t>版本</t>
@@ -1010,8 +800,8 @@
     <col min="21" max="21" width="18.25" customWidth="1" style="1"/>
     <col min="22" max="23" width="9" customWidth="1" style="1"/>
     <col min="24" max="24" width="18.25" customWidth="1" style="1"/>
-    <col min="25" max="30" width="9" customWidth="1" style="1"/>
-    <col min="31" max="16384" width="9" customWidth="1" style="1"/>
+    <col min="25" max="31" width="9" customWidth="1" style="1"/>
+    <col min="32" max="16384" width="9" customWidth="1" style="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1019,165 +809,165 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>151</v>
+        <v>81</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>152</v>
+        <v>82</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>153</v>
+        <v>83</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>154</v>
+        <v>84</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>155</v>
+        <v>85</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>156</v>
+        <v>86</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>157</v>
+        <v>87</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>158</v>
+        <v>88</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>159</v>
+        <v>89</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>160</v>
+        <v>90</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>161</v>
+        <v>91</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>162</v>
+        <v>92</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>163</v>
+        <v>93</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>164</v>
+        <v>94</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>165</v>
+        <v>95</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>166</v>
+        <v>96</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>167</v>
+        <v>97</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>168</v>
+        <v>98</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>169</v>
+        <v>99</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>170</v>
+        <v>100</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>171</v>
+        <v>101</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>172</v>
+        <v>102</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>173</v>
+        <v>103</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>174</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>175</v>
+        <v>105</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>176</v>
+        <v>106</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>177</v>
+        <v>107</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>178</v>
+        <v>108</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>179</v>
+        <v>109</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>180</v>
+        <v>110</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>181</v>
+        <v>111</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>182</v>
+        <v>112</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>183</v>
+        <v>113</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>184</v>
+        <v>114</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>185</v>
+        <v>115</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>186</v>
+        <v>116</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>187</v>
+        <v>117</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>188</v>
+        <v>118</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>189</v>
+        <v>119</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>190</v>
+        <v>120</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>191</v>
+        <v>121</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>192</v>
+        <v>122</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>193</v>
+        <v>123</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>194</v>
+        <v>124</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>195</v>
+        <v>125</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>196</v>
+        <v>126</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>197</v>
+        <v>127</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>198</v>
+        <v>128</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>199</v>
+        <v>129</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>200</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3">
@@ -1185,19 +975,19 @@
         <v>447</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>201</v>
+        <v>131</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>202</v>
+        <v>132</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>203</v>
+        <v>133</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>204</v>
+        <v>134</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>205</v>
+        <v>135</v>
       </c>
       <c r="G3" s="1">
         <v>15</v>
@@ -1221,25 +1011,25 @@
         <v>30001208</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>206</v>
+        <v>136</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>207</v>
+        <v>137</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>208</v>
+        <v>138</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>209</v>
+        <v>139</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>210</v>
+        <v>140</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>211</v>
+        <v>141</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>212</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1255,7 +1045,7 @@
   <dimension ref="A1:AL24"/>
   <sheetViews>
     <sheetView showFormulas="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1283,8 +1073,8 @@
     <col min="34" max="34" width="13" customWidth="1" style="1"/>
     <col min="35" max="37" width="9" customWidth="1" style="1"/>
     <col min="38" max="38" width="13" customWidth="1" style="1"/>
-    <col min="39" max="44" width="9" customWidth="1" style="1"/>
-    <col min="45" max="16384" width="9" customWidth="1" style="1"/>
+    <col min="39" max="45" width="9" customWidth="1" style="1"/>
+    <col min="46" max="16384" width="9" customWidth="1" style="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1583,2432 +1373,2432 @@
         <v>53</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AE4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AF4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AG4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AH4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AJ4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AK4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AL4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AE5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AF5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AG5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AH5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AJ5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AK5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AL5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AB6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AF6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AG6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AH6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AJ6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AK6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AL6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AB7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AE7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AF7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AG7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AH7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AJ7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AK7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AL7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="X8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AB8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AE8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AF8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AG8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AH8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AJ8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AK8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AL8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="X9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Y9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Z9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AA9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AB9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AE9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AF9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AG9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AH9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AJ9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AK9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AL9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="X10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Z10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AE10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AF10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AG10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AH10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AJ10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AK10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AL10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Z11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AA11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AB11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AE11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AF11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AG11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AH11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AJ11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AK11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AL11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="X12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Z12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AA12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AB12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AC12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AE12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AF12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AG12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AH12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AJ12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AK12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AL12" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Z13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AA13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AB13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AC13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AE13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AF13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AG13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AH13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AJ13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AK13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AL13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="X14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Z14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AA14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AB14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AC14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AE14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AF14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AG14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AH14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AJ14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AK14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AL14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="X15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Z15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AA15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AB15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AC15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AE15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AF15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AG15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AH15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AJ15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AK15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AL15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>91</v>
+        <v>53</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="X16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Z16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AA16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AB16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AC16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AE16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AF16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AG16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AH16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AJ16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AK16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AL16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>93</v>
+        <v>53</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>94</v>
+        <v>53</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="X17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Y17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Z17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AA17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AB17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AC17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AE17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AF17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AG17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AH17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AJ17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AK17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AL17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>96</v>
+        <v>53</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="X18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Z18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AA18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AB18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AC18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AE18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AF18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AG18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AH18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AJ18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AK18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AL18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>99</v>
+        <v>53</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="X19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Y19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Z19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AA19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AB19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AC19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AE19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AF19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AG19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AH19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AJ19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AK19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AL19" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>102</v>
+        <v>53</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>103</v>
+        <v>53</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="X20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Y20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Z20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AA20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AB20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AC20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AE20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AF20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AG20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AH20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AJ20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AK20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AL20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>105</v>
+        <v>53</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>106</v>
+        <v>53</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="X21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Y21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Z21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AA21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AB21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AC21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AE21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AF21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AG21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AH21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AJ21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AK21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AL21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>107</v>
+        <v>71</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>108</v>
+        <v>53</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>109</v>
+        <v>53</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="X22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Y22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Z22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AA22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AB22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AC22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AE22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AF22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AG22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AH22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AJ22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AK22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AL22" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>110</v>
+        <v>72</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>111</v>
+        <v>53</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>112</v>
+        <v>53</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="X23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Y23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Z23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AA23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AB23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AC23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AE23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AF23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AG23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AH23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AJ23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AK23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AL23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>113</v>
+        <v>73</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>114</v>
+        <v>53</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>115</v>
+        <v>53</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="T24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="X24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Y24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Z24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AA24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AB24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AC24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AD24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AE24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AF24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AG24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AH24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AJ24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AK24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AL24" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -4032,10 +3822,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4046,178 +3836,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>116</v>
+        <v>74</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>117</v>
+        <v>75</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>118</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>119</v>
+        <v>77</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>120</v>
+        <v>78</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>149</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>